<commit_message>
Finished Week2 Lesson 1, but skipped Week1 Lesson4 PostClass
</commit_message>
<xml_diff>
--- a/SA 1/Week1/L1/Exercise1.xlsx
+++ b/SA 1/Week1/L1/Exercise1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitRepo\MUFYICT\SA 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepo\MUFYICT\SA 1\Week1\L1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16457" windowHeight="5546" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16455" windowHeight="5550"/>
   </bookViews>
   <sheets>
     <sheet name="Student Assignment" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>STUDENT ASSIGNMENT (JAN 2018)</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Wage</t>
+  </si>
+  <si>
+    <t>Distinction?</t>
   </si>
 </sst>
 </file>
@@ -608,15 +611,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I18"/>
+  <dimension ref="A2:J18"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="12" t="s">
         <v>0</v>
@@ -625,8 +631,8 @@
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="1:9" ht="58.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -654,8 +660,11 @@
       <c r="I4" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -687,8 +696,12 @@
         <f>IF(E5&gt;50,"Pass","Fail")</f>
         <v>Pass</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J5" s="2" t="str">
+        <f>IF(AND(G5="Pass",H5="Pass",I5="Pass"),"Distinction","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>6</v>
       </c>
@@ -720,8 +733,12 @@
         <f t="shared" ref="I6:I11" si="3">IF(E6&gt;50,"Pass","Fail")</f>
         <v>Fail</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J6" s="2" t="str">
+        <f t="shared" ref="J6:J12" si="4">IF(AND(G6="Pass",H6="Pass",I6="Pass"),"Distinction","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -753,8 +770,12 @@
         <f t="shared" si="3"/>
         <v>Pass</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J7" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -786,8 +807,12 @@
         <f t="shared" si="3"/>
         <v>Pass</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J8" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>Distinction</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -819,8 +844,12 @@
         <f t="shared" si="3"/>
         <v>Fail</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J9" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>4</v>
       </c>
@@ -852,8 +881,12 @@
         <f t="shared" si="3"/>
         <v>Pass</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J10" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>Distinction</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>5</v>
       </c>
@@ -885,8 +918,12 @@
         <f t="shared" si="3"/>
         <v>Pass</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J11" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>Distinction</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -918,11 +955,15 @@
         <f>IF(E12&gt;50,"Pass","Fail")</f>
         <v>Pass</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J12" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>Distinction</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
@@ -931,15 +972,15 @@
         <v>90</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" ref="D14:E14" si="4">MAX(D5:D12)</f>
+        <f t="shared" ref="D14:E14" si="5">MAX(D5:D12)</f>
         <v>100</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
@@ -948,15 +989,15 @@
         <v>34</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" ref="D15:E15" si="5">MIN(D5:D12)</f>
+        <f t="shared" ref="D15:E15" si="6">MIN(D5:D12)</f>
         <v>10</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
@@ -965,15 +1006,15 @@
         <v>66.875</v>
       </c>
       <c r="D16" s="8">
-        <f t="shared" ref="D16:E16" si="6">AVERAGE(D5:D12)</f>
+        <f t="shared" ref="D16:E16" si="7">AVERAGE(D5:D12)</f>
         <v>62.75</v>
       </c>
       <c r="E16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>69.375</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
@@ -982,15 +1023,15 @@
         <v>8</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" ref="D17:E17" si="7">COUNTA(D5:D12)</f>
+        <f t="shared" ref="D17:E17" si="8">COUNTA(D5:D12)</f>
         <v>8</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
@@ -999,11 +1040,11 @@
         <v>8</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" ref="D18:E18" si="8">COUNTA(D5:D12)</f>
+        <f t="shared" ref="D18:E18" si="9">COUNTA(D5:D12)</f>
         <v>8</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -1026,16 +1067,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
@@ -1049,7 +1090,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -1064,7 +1105,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>25</v>
       </c>
@@ -1079,7 +1120,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -1094,7 +1135,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>26</v>
       </c>
@@ -1109,13 +1150,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="11"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>28</v>
       </c>
@@ -1123,7 +1164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>

</xml_diff>